<commit_message>
Updated code - package has been restructured to make it more intuitive.
</commit_message>
<xml_diff>
--- a/notebooks/Queueing theory - D D 1 example.xlsx
+++ b/notebooks/Queueing theory - D D 1 example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE03D6-AD6C-4F5C-A767-AF6FF2A2A032}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB7D095-FDFF-4468-9DF6-A8042943E1AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC2DE56-B1A7-4720-AEDB-7DC668B2912F}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,23 +649,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3">
-        <f t="shared" ref="C2:C32" si="0">F2+G2</f>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D2" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E2" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F2" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G2" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3">
         <v>80</v>
@@ -676,24 +675,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <f>D3-D2</f>
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="E3" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H3" s="3">
         <v>80</v>
@@ -704,21 +701,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <f>D4-D3</f>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3">
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="E4" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F4" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -732,24 +727,22 @@
         <v>0</v>
       </c>
       <c r="B5" s="3">
-        <f t="shared" ref="B5:B32" si="1">D5-D4</f>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3">
         <v>80</v>
@@ -760,24 +753,22 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D6" s="3">
-        <v>9</v>
+        <v>216</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G6" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H6" s="3">
         <v>90</v>
@@ -788,24 +779,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="D7" s="3">
-        <v>12</v>
+        <v>288</v>
       </c>
       <c r="E7" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G7" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H7" s="3">
         <v>100</v>
@@ -816,24 +805,22 @@
         <v>0</v>
       </c>
       <c r="B8" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D8" s="3">
-        <v>16</v>
+        <v>384</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G8" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H8" s="3">
         <v>80</v>
@@ -844,24 +831,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D9" s="3">
-        <v>18</v>
+        <v>432</v>
       </c>
       <c r="E9" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F9" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G9" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H9" s="3">
         <v>80</v>
@@ -872,24 +857,22 @@
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D10" s="3">
-        <v>19</v>
+        <v>456</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G10" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H10" s="3">
         <v>90</v>
@@ -900,24 +883,22 @@
         <v>0</v>
       </c>
       <c r="B11" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D11" s="3">
-        <v>23</v>
+        <v>552</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H11" s="3">
         <v>80</v>
@@ -928,21 +909,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3">
-        <v>23</v>
+        <v>552</v>
       </c>
       <c r="E12" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F12" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -956,24 +935,22 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D13" s="3">
-        <v>24</v>
+        <v>576</v>
       </c>
       <c r="E13" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G13" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H13" s="3">
         <v>160</v>
@@ -984,24 +961,22 @@
         <v>4</v>
       </c>
       <c r="B14" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D14" s="3">
-        <v>29</v>
+        <v>696</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G14" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H14" s="3">
         <v>90</v>
@@ -1012,24 +987,22 @@
         <v>0</v>
       </c>
       <c r="B15" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C15" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D15" s="3">
-        <v>30</v>
+        <v>720</v>
       </c>
       <c r="E15" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F15" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G15" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H15" s="3">
         <v>80</v>
@@ -1040,24 +1013,22 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D16" s="3">
-        <v>34</v>
+        <v>816</v>
       </c>
       <c r="E16" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F16" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G16" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H16" s="3">
         <v>80</v>
@@ -1068,24 +1039,22 @@
         <v>0</v>
       </c>
       <c r="B17" s="3">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="C17" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D17" s="3">
-        <v>37</v>
+        <v>888</v>
       </c>
       <c r="E17" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F17" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G17" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H17" s="3">
         <v>80</v>
@@ -1096,24 +1065,22 @@
         <v>4</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D18" s="3">
-        <v>39</v>
+        <v>936</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G18" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H18" s="3">
         <v>90</v>
@@ -1124,21 +1091,19 @@
         <v>2</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3">
-        <v>41</v>
+        <v>984</v>
       </c>
       <c r="E19" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F19" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -1152,24 +1117,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="D20" s="3">
-        <v>42</v>
+        <v>1008</v>
       </c>
       <c r="E20" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F20" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G20" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H20" s="3">
         <v>100</v>
@@ -1180,24 +1143,22 @@
         <v>0</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D21" s="3">
-        <v>44</v>
+        <v>1056</v>
       </c>
       <c r="E21" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F21" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G21" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H21" s="3">
         <v>80</v>
@@ -1208,24 +1169,22 @@
         <v>4</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D22" s="3">
-        <v>49</v>
+        <v>1176</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G22" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H22" s="3">
         <v>90</v>
@@ -1236,24 +1195,22 @@
         <v>5</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D23" s="3">
-        <v>50</v>
+        <v>1200</v>
       </c>
       <c r="E23" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F23" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G23" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H23" s="3">
         <v>80</v>
@@ -1264,24 +1221,22 @@
         <v>0</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C24" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3">
-        <v>51</v>
+        <v>1224</v>
       </c>
       <c r="E24" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F24" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G24" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H24" s="3">
         <v>80</v>
@@ -1292,24 +1247,22 @@
         <v>0</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="C25" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D25" s="3">
-        <v>58</v>
+        <v>1392</v>
       </c>
       <c r="E25" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G25" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H25" s="3">
         <v>80</v>
@@ -1320,21 +1273,19 @@
         <v>2</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D26" s="3">
-        <v>59</v>
+        <v>1416</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F26" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G26" s="3">
         <v>0</v>
@@ -1348,24 +1299,22 @@
         <v>4</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="D27" s="3">
-        <v>59</v>
+        <v>1416</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
       <c r="F27" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G27" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H27" s="3">
         <v>90</v>
@@ -1376,24 +1325,22 @@
         <v>0</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D28" s="3">
-        <v>65</v>
+        <v>1560</v>
       </c>
       <c r="E28" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F28" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="G28" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H28" s="3">
         <v>80</v>
@@ -1404,24 +1351,22 @@
         <v>5</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>120</v>
       </c>
       <c r="D29" s="3">
-        <v>66</v>
+        <v>1584</v>
       </c>
       <c r="E29" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F29" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G29" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="H29" s="3">
         <v>80</v>
@@ -1432,24 +1377,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="D30" s="3">
-        <v>72</v>
+        <v>1728</v>
       </c>
       <c r="E30" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F30" s="3">
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="G30" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H30" s="3">
         <v>100</v>
@@ -1460,24 +1403,22 @@
         <v>3</v>
       </c>
       <c r="B31" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <v>288</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3">
-        <v>84</v>
+        <v>2016</v>
       </c>
       <c r="E31" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F31" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G31" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H31" s="3">
         <v>160</v>
@@ -1488,24 +1429,22 @@
         <v>3</v>
       </c>
       <c r="B32" s="3">
-        <f t="shared" si="1"/>
-        <v>60</v>
+        <v>1440</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>96</v>
       </c>
       <c r="D32" s="3">
-        <v>144</v>
+        <v>3456</v>
       </c>
       <c r="E32" s="3">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="F32" s="3">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G32" s="3">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H32" s="3">
         <v>160</v>

</xml_diff>